<commit_message>
Fix vid tomma rader i excellen på deltagare
</commit_message>
<xml_diff>
--- a/mallar/import/TDB_SM_2018_Export_002_2018_08_17 (1).xlsx
+++ b/mallar/import/TDB_SM_2018_Export_002_2018_08_17 (1).xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11B1D9B6-B93D-44C0-9700-8C1058BC0B97}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882F316B-C825-4A31-B181-561E2445591D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16185" windowHeight="5198" xr2:uid="{9D7E8EEF-4AF9-4E19-AACF-EC41985FBDB0}"/>
   </bookViews>
   <sheets>
-    <sheet name="ekipage" sheetId="1" r:id="rId1"/>
-    <sheet name="klasser" sheetId="2" r:id="rId2"/>
-    <sheet name="linförare" sheetId="3" r:id="rId3"/>
+    <sheet name="Ekipage" sheetId="1" r:id="rId1"/>
+    <sheet name="Klasser" sheetId="2" r:id="rId2"/>
+    <sheet name="Linförare" sheetId="3" r:id="rId3"/>
     <sheet name="hästar" sheetId="4" r:id="rId4"/>
     <sheet name="klubbar" sheetId="5" r:id="rId5"/>
-    <sheet name="voltigörer" sheetId="6" r:id="rId6"/>
+    <sheet name="Tävlande" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3244,7 +3244,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4045,7 +4045,7 @@
   <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>